<commit_message>
Added outputHeadingsAs paramter when exporting to Excel.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\pivottabler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D094680-E769-4182-8F98-D66D95ED60DB}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E6F2A5-11FF-4436-A83E-FA30762339FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{8F97058A-2917-4304-96C6-C09198596679}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
   <si>
     <t>integer</t>
   </si>
@@ -161,6 +161,9 @@
   <si>
     <t xml:space="preserve">In NEWS.md, move the examples and refer to the Appendix.
 </t>
+  </si>
+  <si>
+    <t>Add default formats for dates and date times if not specified.</t>
   </si>
 </sst>
 </file>
@@ -552,10 +555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BFBB9C-794B-48B7-8168-9DF05A51AB93}">
-  <dimension ref="B1:H27"/>
+  <dimension ref="B1:I27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -570,12 +573,12 @@
     <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -589,38 +592,38 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="F3" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="2" t="s">
+      <c r="H3" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="C4" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="D4" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="E4" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F4" s="2" t="s">
@@ -633,17 +636,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F5" s="2" t="s">
@@ -656,17 +659,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F6" s="2" t="s">
@@ -679,17 +682,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F7" s="2" t="s">
@@ -702,17 +705,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F8" s="2" t="s">
@@ -725,17 +728,17 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E9" s="3" t="s">
+      <c r="E9" s="2" t="s">
         <v>20</v>
       </c>
       <c r="F9" s="2" t="s">
@@ -748,15 +751,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
@@ -764,23 +767,28 @@
         <v>33</v>
       </c>
       <c r="E12" s="2"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="G12" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="H12" s="3"/>
+      <c r="I12" s="3"/>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>

</xml_diff>

<commit_message>
Added the ability to specify style settings when adding data groups and defining calculations.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\pivottabler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62E6F2A5-11FF-4436-A83E-FA30762339FF}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBC72A3-1069-4B55-ACC2-6D0D07E5479E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{8F97058A-2917-4304-96C6-C09198596679}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
   <si>
     <t>integer</t>
   </si>
@@ -163,7 +163,19 @@
 </t>
   </si>
   <si>
-    <t>Add default formats for dates and date times if not specified.</t>
+    <t>Add note to the docs that for excel export, outputting values as rawValue for dates/posixct will cause a number to appear.</t>
+  </si>
+  <si>
+    <t>Issue 9:  Support changing PivotDataGroup caption</t>
+  </si>
+  <si>
+    <t>Issue 3:  defineCalculation(filters) should be able to replace filters, not just combine with AND</t>
+  </si>
+  <si>
+    <t>Issue 1:  calculationType "value" should work with totals</t>
+  </si>
+  <si>
+    <t>Add quick pivot tests (see trello).</t>
   </si>
 </sst>
 </file>
@@ -555,10 +567,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BFBB9C-794B-48B7-8168-9DF05A51AB93}">
-  <dimension ref="B1:I27"/>
+  <dimension ref="B1:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="G24" sqref="G24:G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -573,12 +585,12 @@
     <col min="8" max="8" width="27.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
       <c r="E1" s="1"/>
     </row>
-    <row r="2" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B2" s="1" t="s">
         <v>22</v>
       </c>
@@ -592,7 +604,7 @@
       </c>
       <c r="G2" s="1"/>
     </row>
-    <row r="3" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="1" t="s">
         <v>6</v>
@@ -613,7 +625,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="4" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="1" t="s">
         <v>0</v>
       </c>
@@ -636,7 +648,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="5" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
@@ -659,7 +671,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
@@ -682,7 +694,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B7" s="1" t="s">
         <v>2</v>
       </c>
@@ -705,7 +717,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B8" s="1" t="s">
         <v>4</v>
       </c>
@@ -728,7 +740,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B9" s="1" t="s">
         <v>5</v>
       </c>
@@ -751,15 +763,15 @@
         <v>21</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="1"/>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="1" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C12" s="2" t="s">
         <v>29</v>
       </c>
@@ -767,28 +779,23 @@
         <v>33</v>
       </c>
       <c r="E12" s="2"/>
-      <c r="G12" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C13" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C14" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C15" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="C16" s="2" t="s">
         <v>25</v>
       </c>
@@ -831,57 +838,98 @@
       <c r="G19" s="2"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C21" s="3"/>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>39</v>
+        <v>49</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
-      <c r="F23" s="3"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
-      <c r="F24" s="3"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="3" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
-      <c r="F25" s="3"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="3" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
-      <c r="F26" s="3"/>
-    </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="4" t="s">
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B29" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B30" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B31" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B32" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C32" s="3"/>
+      <c r="D32" s="3"/>
+      <c r="E32" s="3"/>
+      <c r="F32" s="3"/>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
PivotFilterOverrides class added providing more options for changing filter criteria as part of calculations (e.g. for percentage of row/column/grand total).
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\pivottabler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABBC72A3-1069-4B55-ACC2-6D0D07E5479E}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EC04CD-F776-44E4-9B47-375DF77303FD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{8F97058A-2917-4304-96C6-C09198596679}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
   <si>
     <t>integer</t>
   </si>
@@ -151,9 +151,6 @@
   </si>
   <si>
     <t>review the content of all of the existing vignettes and ensure the below are either added in existing vignettes or a new FAQ vignette.</t>
-  </si>
-  <si>
-    <t>(1) Data type support, (2) data type formatting, (3) Dealing with columns with illegal names, (4) New export options</t>
   </si>
   <si>
     <t xml:space="preserve">  If the return value of the above is FALSE, then still want to apply styling, etc.</t>
@@ -172,10 +169,19 @@
     <t>Issue 3:  defineCalculation(filters) should be able to replace filters, not just combine with AND</t>
   </si>
   <si>
-    <t>Issue 1:  calculationType "value" should work with totals</t>
-  </si>
-  <si>
-    <t>Add quick pivot tests (see trello).</t>
+    <t>Add quick pivot tests (see trello), add tests for specifying style info (baseStyleName, styleDeclarations) upfront, add tests for filteroverrides</t>
+  </si>
+  <si>
+    <t>Follow normal dev workflow.</t>
+  </si>
+  <si>
+    <t>Release as v1.0 to CRAN.</t>
+  </si>
+  <si>
+    <t>(5) Upfront styling, (6) overriding filters as part of calculations.</t>
+  </si>
+  <si>
+    <t>(1) Data type support, (2) data type formatting, (3) Dealing with columns with illegal names, (4) New export options,</t>
   </si>
 </sst>
 </file>
@@ -567,10 +573,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BFBB9C-794B-48B7-8168-9DF05A51AB93}">
-  <dimension ref="B1:H33"/>
+  <dimension ref="B1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G24" sqref="G24:G25"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -823,7 +829,7 @@
         <v>26</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="G18" s="2"/>
       <c r="H18" s="2"/>
@@ -847,39 +853,42 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+      <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="C25" s="3"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
-    </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C26" s="3"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
+      <c r="B25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -888,7 +897,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -897,7 +906,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>41</v>
+        <v>51</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -906,7 +915,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>42</v>
+        <v>50</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -915,7 +924,7 @@
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B32" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -924,12 +933,30 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="4" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Changing pivot data group captions.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\pivottabler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3EC04CD-F776-44E4-9B47-375DF77303FD}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C67D966-332A-407E-ADD8-78435327DE86}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{8F97058A-2917-4304-96C6-C09198596679}"/>
   </bookViews>
@@ -576,7 +576,7 @@
   <dimension ref="B1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -862,12 +862,12 @@
       <c r="G23" s="3"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C24" s="3"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">

</xml_diff>

<commit_message>
Additional options for filter overriding.
</commit_message>
<xml_diff>
--- a/ToDo.xlsx
+++ b/ToDo.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\R\pivottabler\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C67D966-332A-407E-ADD8-78435327DE86}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A7E8495-23A9-4BEB-8AD2-072E75238ECA}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="21570" windowHeight="7680" xr2:uid="{8F97058A-2917-4304-96C6-C09198596679}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="53">
   <si>
     <t>integer</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>(1) Data type support, (2) data type formatting, (3) Dealing with columns with illegal names, (4) New export options,</t>
+  </si>
+  <si>
+    <t>test each of the new data type examples with visual totals.</t>
   </si>
 </sst>
 </file>
@@ -573,11 +576,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08BFBB9C-794B-48B7-8168-9DF05A51AB93}">
-  <dimension ref="B1:H35"/>
+  <dimension ref="B1:H36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -878,17 +879,17 @@
       <c r="E25" s="2"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="3" t="s">
-        <v>40</v>
+        <v>52</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -897,7 +898,7 @@
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C29" s="3"/>
       <c r="D29" s="3"/>
@@ -906,7 +907,7 @@
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -915,7 +916,7 @@
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="C31" s="3"/>
       <c r="D31" s="3"/>
@@ -923,8 +924,8 @@
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="4" t="s">
-        <v>43</v>
+      <c r="B32" s="3" t="s">
+        <v>50</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -933,7 +934,7 @@
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
@@ -942,7 +943,7 @@
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -951,12 +952,21 @@
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="4" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>